<commit_message>
CleanUp for Sim C
Cleaned and commented the section in MAKE3DOF where edits were made to determine simulation parameter constant for the motor.
</commit_message>
<xml_diff>
--- a/S3_VMU/Master_Model_3DOF/Raw_Data/PER25_OU27.xlsx
+++ b/S3_VMU/Master_Model_3DOF/Raw_Data/PER25_OU27.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\droli\Documents\GitHub\SimscapeModel\S3_VMU\Master_Model_3DOF\Raw_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50DFBC98-9696-4E42-AD1D-5FA0B66822BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C098031F-DCD1-4E49-858D-4E52093E6380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5105A7BF-846E-4EF7-B817-7E9624B68BB3}"/>
   </bookViews>
@@ -115,6 +115,2731 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v> Main</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> InverterA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> INVA_CRIT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> AMK_ActualTorque</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$5:$B$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="157"/>
+                <c:pt idx="0">
+                  <c:v>7.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>148.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>166.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>167.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>168.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>168</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>168.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>170.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>168.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>165.2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>166.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>166.3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>159.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>166.4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>159.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>170.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>167.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>165.6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>156.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>130.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>97.9</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>81.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>53.3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36.6</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>37.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>36.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35.4</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>37.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>37.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>38.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>38.9</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>37.1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>36.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>36.6</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>36.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>35.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>38.4</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>37.5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>43.6</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>48.5</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>50.8</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>50.6</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>53.1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57.1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>70.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>73.5</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>90.2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>94.3</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>94.3</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>95.1</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>101.9</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>94.8</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>95.9</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>94.4</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>94.3</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>94.7</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>96.4</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>95.6</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96.5</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>95.3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>96.8</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>96.3</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>97.2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>95.7</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>95.2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>103.4</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>118.4</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>123.1</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>123.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>128.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>133.5</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>145.4</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>147.4</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>143.9</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>148.5</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>147.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>153</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>149.4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>149.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>147.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>150.1</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>147.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>150.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>150.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>149.9</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>151.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>149.1</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>147.1</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>149.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>137</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>143.5</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>150.5</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>148.9</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>148.1</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>148.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>149.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>148.4</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>150.5</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>151.1</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>151.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>149.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>150.1</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>150.9</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>151.5</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>148.4</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>157.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>157.4</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>153.5</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>152.5</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>151.5</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>149.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>149.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>150.6</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>151.9</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>152.4</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>154.9</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>147.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>152.1</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>151.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>151.9</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>149.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>146.80000000000001</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>150.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>144.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>147.4</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>147.9</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>136.69999999999999</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>124.8</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>125.9</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>85.3</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>67.8</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>49.1</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>45.7</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>38.1</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>31.4</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>-0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-CC0D-44A8-963A-F748A6251A70}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900734271"/>
+        <c:axId val="900730911"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="900734271"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900730911"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="900730911"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900734271"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v> Main</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> InverterA</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> INVA_CRIT</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> AMK_DisplayOverloadInverter</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$5:$C$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="157"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-69A1-4D93-8C70-9741843200DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900740031"/>
+        <c:axId val="857441647"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="900740031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="857441647"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="857441647"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900740031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D08E28CD-5632-05C3-ED62-BD77E7CA473D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07ECD7AD-77DF-B273-E58F-EB545DF20271}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -437,7 +3162,7 @@
   <dimension ref="A1:C161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D168" sqref="D168"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,5 +4940,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>